<commit_message>
Updated to handle overlapped courses, false courses
</commit_message>
<xml_diff>
--- a/course_plan_excel_frame/Information and Communication Technology.xlsx
+++ b/course_plan_excel_frame/Information and Communication Technology.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29311"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A21D45E-717F-45FD-B2F4-50CFE588A8C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{636DBCDF-77CE-41D6-92B9-3142BDB52592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="29">
   <si>
     <t>1. General Education</t>
   </si>
@@ -111,72 +111,6 @@
     <t>60 Credits</t>
   </si>
   <si>
-    <t>ITE201</t>
-  </si>
-  <si>
-    <t>ICT101</t>
-  </si>
-  <si>
-    <t>ICT102</t>
-  </si>
-  <si>
-    <t>ICT103</t>
-  </si>
-  <si>
-    <t>ICT110</t>
-  </si>
-  <si>
-    <t>ICT202</t>
-  </si>
-  <si>
-    <t>ICT209</t>
-  </si>
-  <si>
-    <t>ICT210</t>
-  </si>
-  <si>
-    <t>ICT211</t>
-  </si>
-  <si>
-    <t>ICT212</t>
-  </si>
-  <si>
-    <t>ICT213</t>
-  </si>
-  <si>
-    <t>ICT215</t>
-  </si>
-  <si>
-    <t>ICT301</t>
-  </si>
-  <si>
-    <t>ICT302</t>
-  </si>
-  <si>
-    <t>ICT304</t>
-  </si>
-  <si>
-    <t>ICT305</t>
-  </si>
-  <si>
-    <t>ICT401</t>
-  </si>
-  <si>
-    <t>ICT402</t>
-  </si>
-  <si>
-    <t>ICT493</t>
-  </si>
-  <si>
-    <t>ICT494</t>
-  </si>
-  <si>
-    <t>ICT495</t>
-  </si>
-  <si>
-    <t>ICT498</t>
-  </si>
-  <si>
     <t>2.3 Major Elective Requirements</t>
   </si>
   <si>
@@ -184,6 +118,9 @@
   </si>
   <si>
     <t>6 Credits</t>
+  </si>
+  <si>
+    <t>False Courses</t>
   </si>
 </sst>
 </file>
@@ -194,7 +131,7 @@
     <numFmt numFmtId="187" formatCode="m/d"/>
     <numFmt numFmtId="188" formatCode="m/yyyy"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -243,8 +180,21 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Mono"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -293,8 +243,14 @@
         <bgColor rgb="FFD9EAD3"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -494,12 +450,64 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -693,29 +701,14 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -726,21 +719,48 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -960,10 +980,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F273"/>
+  <dimension ref="A1:F269"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H53" sqref="H53"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78:E79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="18" customHeight="1"/>
@@ -980,12 +1000,12 @@
       <c r="E1" s="42"/>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A2" s="73" t="s">
+      <c r="A2" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
       <c r="E2" s="26" t="s">
         <v>1</v>
       </c>
@@ -998,12 +1018,12 @@
       <c r="E3" s="28"/>
     </row>
     <row r="4" spans="1:6" s="1" customFormat="1" ht="18" customHeight="1">
-      <c r="A4" s="75" t="s">
+      <c r="A4" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="76"/>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
+      <c r="B4" s="66"/>
+      <c r="C4" s="66"/>
+      <c r="D4" s="66"/>
       <c r="E4" s="4" t="s">
         <v>3</v>
       </c>
@@ -1044,10 +1064,10 @@
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" ht="18" customHeight="1">
-      <c r="A8" s="65" t="s">
+      <c r="A8" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="66"/>
+      <c r="B8" s="73"/>
       <c r="C8" s="47">
         <f>SUMIF(D6:D7,"&lt;&gt;",C6:C7)</f>
         <v>0</v>
@@ -1065,12 +1085,12 @@
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" ht="18" customHeight="1">
-      <c r="A10" s="77" t="s">
+      <c r="A10" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="76"/>
-      <c r="C10" s="76"/>
-      <c r="D10" s="76"/>
+      <c r="B10" s="66"/>
+      <c r="C10" s="66"/>
+      <c r="D10" s="66"/>
       <c r="E10" s="12" t="s">
         <v>10</v>
       </c>
@@ -1129,10 +1149,10 @@
       <c r="E15" s="18"/>
     </row>
     <row r="16" spans="1:6" ht="18" customHeight="1">
-      <c r="A16" s="67" t="s">
+      <c r="A16" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="68"/>
+      <c r="B16" s="75"/>
       <c r="C16" s="49">
         <f>SUMIF(D12:D15,"&lt;&gt;",C12:C15)</f>
         <v>0</v>
@@ -1148,12 +1168,12 @@
       <c r="E17" s="11"/>
     </row>
     <row r="18" spans="1:6" ht="18" customHeight="1">
-      <c r="A18" s="78" t="s">
+      <c r="A18" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="76"/>
-      <c r="C18" s="76"/>
-      <c r="D18" s="76"/>
+      <c r="B18" s="66"/>
+      <c r="C18" s="66"/>
+      <c r="D18" s="66"/>
       <c r="E18" s="19" t="s">
         <v>12</v>
       </c>
@@ -1248,10 +1268,10 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="18" customHeight="1">
-      <c r="A26" s="69" t="s">
+      <c r="A26" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="70"/>
+      <c r="B26" s="77"/>
       <c r="C26" s="56">
         <f>SUMIF(D20:D25,"&lt;&gt;",C20:C25)</f>
         <v>0</v>
@@ -1268,12 +1288,12 @@
       <c r="E27" s="11"/>
     </row>
     <row r="28" spans="1:6" s="27" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A28" s="73" t="s">
+      <c r="A28" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="74"/>
-      <c r="C28" s="74"/>
-      <c r="D28" s="74"/>
+      <c r="B28" s="69"/>
+      <c r="C28" s="69"/>
+      <c r="D28" s="69"/>
       <c r="E28" s="26" t="s">
         <v>20</v>
       </c>
@@ -1287,12 +1307,12 @@
       <c r="E29" s="28"/>
     </row>
     <row r="30" spans="1:6" ht="18" customHeight="1">
-      <c r="A30" s="75" t="s">
+      <c r="A30" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="B30" s="76"/>
-      <c r="C30" s="76"/>
-      <c r="D30" s="76"/>
+      <c r="B30" s="66"/>
+      <c r="C30" s="66"/>
+      <c r="D30" s="66"/>
       <c r="E30" s="4" t="s">
         <v>22</v>
       </c>
@@ -1341,10 +1361,10 @@
       <c r="E34" s="29"/>
     </row>
     <row r="35" spans="1:6" ht="18" customHeight="1">
-      <c r="A35" s="65" t="s">
+      <c r="A35" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="B35" s="66"/>
+      <c r="B35" s="73"/>
       <c r="C35" s="47">
         <f>SUMIF(D32:D34,"&lt;&gt;",C32:C34)</f>
         <v>0</v>
@@ -1360,12 +1380,12 @@
       <c r="E36" s="11"/>
     </row>
     <row r="37" spans="1:6" ht="18" customHeight="1">
-      <c r="A37" s="79" t="s">
+      <c r="A37" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="B37" s="76"/>
-      <c r="C37" s="76"/>
-      <c r="D37" s="76"/>
+      <c r="B37" s="66"/>
+      <c r="C37" s="66"/>
+      <c r="D37" s="66"/>
       <c r="E37" s="30" t="s">
         <v>24</v>
       </c>
@@ -1390,12 +1410,8 @@
       <c r="A39" s="33">
         <v>1</v>
       </c>
-      <c r="B39" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="C39" s="33">
-        <v>3</v>
-      </c>
+      <c r="B39" s="33"/>
+      <c r="C39" s="33"/>
       <c r="D39" s="33"/>
       <c r="E39" s="34"/>
     </row>
@@ -1403,12 +1419,8 @@
       <c r="A40" s="33">
         <v>2</v>
       </c>
-      <c r="B40" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="C40" s="33">
-        <v>3</v>
-      </c>
+      <c r="B40" s="33"/>
+      <c r="C40" s="33"/>
       <c r="D40" s="33"/>
       <c r="E40" s="34"/>
     </row>
@@ -1416,12 +1428,8 @@
       <c r="A41" s="33">
         <v>3</v>
       </c>
-      <c r="B41" s="33" t="s">
-        <v>27</v>
-      </c>
-      <c r="C41" s="33">
-        <v>3</v>
-      </c>
+      <c r="B41" s="33"/>
+      <c r="C41" s="33"/>
       <c r="D41" s="33"/>
       <c r="E41" s="34"/>
     </row>
@@ -1429,12 +1437,8 @@
       <c r="A42" s="33">
         <v>4</v>
       </c>
-      <c r="B42" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="C42" s="33">
-        <v>3</v>
-      </c>
+      <c r="B42" s="33"/>
+      <c r="C42" s="33"/>
       <c r="D42" s="33"/>
       <c r="E42" s="35"/>
     </row>
@@ -1442,12 +1446,8 @@
       <c r="A43" s="33">
         <v>5</v>
       </c>
-      <c r="B43" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="C43" s="33">
-        <v>3</v>
-      </c>
+      <c r="B43" s="33"/>
+      <c r="C43" s="33"/>
       <c r="D43" s="33"/>
       <c r="E43" s="33"/>
     </row>
@@ -1455,12 +1455,8 @@
       <c r="A44" s="33">
         <v>6</v>
       </c>
-      <c r="B44" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="C44" s="33">
-        <v>3</v>
-      </c>
+      <c r="B44" s="33"/>
+      <c r="C44" s="33"/>
       <c r="D44" s="33"/>
       <c r="E44" s="34"/>
     </row>
@@ -1468,12 +1464,8 @@
       <c r="A45" s="33">
         <v>7</v>
       </c>
-      <c r="B45" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="C45" s="33">
-        <v>3</v>
-      </c>
+      <c r="B45" s="33"/>
+      <c r="C45" s="33"/>
       <c r="D45" s="33"/>
       <c r="E45" s="34"/>
     </row>
@@ -1481,12 +1473,8 @@
       <c r="A46" s="33">
         <v>8</v>
       </c>
-      <c r="B46" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="C46" s="33">
-        <v>3</v>
-      </c>
+      <c r="B46" s="33"/>
+      <c r="C46" s="33"/>
       <c r="D46" s="33"/>
       <c r="E46" s="34"/>
     </row>
@@ -1494,12 +1482,8 @@
       <c r="A47" s="33">
         <v>9</v>
       </c>
-      <c r="B47" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="C47" s="33">
-        <v>3</v>
-      </c>
+      <c r="B47" s="33"/>
+      <c r="C47" s="33"/>
       <c r="D47" s="33"/>
       <c r="E47" s="34"/>
     </row>
@@ -1507,12 +1491,8 @@
       <c r="A48" s="33">
         <v>10</v>
       </c>
-      <c r="B48" s="33" t="s">
-        <v>34</v>
-      </c>
-      <c r="C48" s="33">
-        <v>3</v>
-      </c>
+      <c r="B48" s="33"/>
+      <c r="C48" s="33"/>
       <c r="D48" s="33"/>
       <c r="E48" s="34"/>
     </row>
@@ -1520,12 +1500,8 @@
       <c r="A49" s="33">
         <v>11</v>
       </c>
-      <c r="B49" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="C49" s="33">
-        <v>3</v>
-      </c>
+      <c r="B49" s="33"/>
+      <c r="C49" s="33"/>
       <c r="D49" s="33"/>
       <c r="E49" s="35"/>
     </row>
@@ -1533,12 +1509,8 @@
       <c r="A50" s="33">
         <v>12</v>
       </c>
-      <c r="B50" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="C50" s="33">
-        <v>3</v>
-      </c>
+      <c r="B50" s="33"/>
+      <c r="C50" s="33"/>
       <c r="D50" s="33"/>
       <c r="E50" s="35"/>
     </row>
@@ -1546,12 +1518,8 @@
       <c r="A51" s="33">
         <v>13</v>
       </c>
-      <c r="B51" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="C51" s="33">
-        <v>3</v>
-      </c>
+      <c r="B51" s="33"/>
+      <c r="C51" s="33"/>
       <c r="D51" s="33"/>
       <c r="E51" s="34"/>
     </row>
@@ -1559,12 +1527,8 @@
       <c r="A52" s="33">
         <v>14</v>
       </c>
-      <c r="B52" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="C52" s="33">
-        <v>3</v>
-      </c>
+      <c r="B52" s="33"/>
+      <c r="C52" s="33"/>
       <c r="D52" s="33"/>
       <c r="E52" s="34"/>
     </row>
@@ -1572,12 +1536,8 @@
       <c r="A53" s="33">
         <v>15</v>
       </c>
-      <c r="B53" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="C53" s="33">
-        <v>3</v>
-      </c>
+      <c r="B53" s="33"/>
+      <c r="C53" s="33"/>
       <c r="D53" s="33"/>
       <c r="E53" s="34"/>
     </row>
@@ -1585,12 +1545,8 @@
       <c r="A54" s="33">
         <v>16</v>
       </c>
-      <c r="B54" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="C54" s="33">
-        <v>3</v>
-      </c>
+      <c r="B54" s="33"/>
+      <c r="C54" s="33"/>
       <c r="D54" s="33"/>
       <c r="E54" s="34"/>
     </row>
@@ -1598,12 +1554,8 @@
       <c r="A55" s="33">
         <v>17</v>
       </c>
-      <c r="B55" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="C55" s="33">
-        <v>3</v>
-      </c>
+      <c r="B55" s="33"/>
+      <c r="C55" s="33"/>
       <c r="D55" s="33"/>
       <c r="E55" s="33"/>
     </row>
@@ -1611,12 +1563,8 @@
       <c r="A56" s="33">
         <v>18</v>
       </c>
-      <c r="B56" s="33" t="s">
-        <v>42</v>
-      </c>
-      <c r="C56" s="33">
-        <v>3</v>
-      </c>
+      <c r="B56" s="33"/>
+      <c r="C56" s="33"/>
       <c r="D56" s="33"/>
       <c r="E56" s="33"/>
     </row>
@@ -1624,12 +1572,8 @@
       <c r="A57" s="36">
         <v>19</v>
       </c>
-      <c r="B57" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="C57" s="36">
-        <v>1</v>
-      </c>
+      <c r="B57" s="36"/>
+      <c r="C57" s="36"/>
       <c r="D57" s="36"/>
       <c r="E57" s="36"/>
     </row>
@@ -1637,12 +1581,8 @@
       <c r="A58" s="36">
         <v>20</v>
       </c>
-      <c r="B58" s="36" t="s">
-        <v>44</v>
-      </c>
-      <c r="C58" s="36">
-        <v>2</v>
-      </c>
+      <c r="B58" s="36"/>
+      <c r="C58" s="36"/>
       <c r="D58" s="36"/>
       <c r="E58" s="36"/>
     </row>
@@ -1650,12 +1590,8 @@
       <c r="A59" s="36">
         <v>21</v>
       </c>
-      <c r="B59" s="36" t="s">
-        <v>45</v>
-      </c>
-      <c r="C59" s="36">
-        <v>3</v>
-      </c>
+      <c r="B59" s="36"/>
+      <c r="C59" s="36"/>
       <c r="D59" s="36"/>
       <c r="E59" s="36"/>
     </row>
@@ -1663,20 +1599,16 @@
       <c r="A60" s="55">
         <v>22</v>
       </c>
-      <c r="B60" s="55" t="s">
-        <v>46</v>
-      </c>
-      <c r="C60" s="55">
-        <v>6</v>
-      </c>
+      <c r="B60" s="55"/>
+      <c r="C60" s="55"/>
       <c r="D60" s="33"/>
       <c r="E60" s="33"/>
     </row>
     <row r="61" spans="1:6" ht="18" customHeight="1">
-      <c r="A61" s="71" t="s">
+      <c r="A61" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="B61" s="72"/>
+      <c r="B61" s="79"/>
       <c r="C61" s="57">
         <f>SUMIF(D39:D60,"&lt;&gt;",C39:C60)</f>
         <v>0</v>
@@ -1692,12 +1624,12 @@
       <c r="E62" s="11"/>
     </row>
     <row r="63" spans="1:6" ht="18" customHeight="1">
-      <c r="A63" s="78" t="s">
-        <v>47</v>
-      </c>
-      <c r="B63" s="76"/>
-      <c r="C63" s="76"/>
-      <c r="D63" s="76"/>
+      <c r="A63" s="65" t="s">
+        <v>25</v>
+      </c>
+      <c r="B63" s="66"/>
+      <c r="C63" s="66"/>
+      <c r="D63" s="66"/>
       <c r="E63" s="19" t="s">
         <v>12</v>
       </c>
@@ -1764,10 +1696,10 @@
       <c r="E69" s="23"/>
     </row>
     <row r="70" spans="1:6" ht="18" customHeight="1">
-      <c r="A70" s="69" t="s">
+      <c r="A70" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="B70" s="70"/>
+      <c r="B70" s="77"/>
       <c r="C70" s="56">
         <f>SUMIF(D65:D69,"&lt;&gt;",C65:C69)</f>
         <v>0</v>
@@ -1783,14 +1715,14 @@
       <c r="E71" s="11"/>
     </row>
     <row r="72" spans="1:6" ht="18" customHeight="1">
-      <c r="A72" s="80" t="s">
-        <v>48</v>
-      </c>
-      <c r="B72" s="76"/>
-      <c r="C72" s="76"/>
-      <c r="D72" s="76"/>
+      <c r="A72" s="67" t="s">
+        <v>26</v>
+      </c>
+      <c r="B72" s="66"/>
+      <c r="C72" s="66"/>
+      <c r="D72" s="66"/>
       <c r="E72" s="37" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="F72" s="1"/>
     </row>
@@ -1846,10 +1778,28 @@
       <c r="E77" s="25"/>
     </row>
     <row r="78" spans="1:6" ht="18" customHeight="1">
-      <c r="E78" s="25"/>
+      <c r="A78" s="81" t="s">
+        <v>28</v>
+      </c>
+      <c r="B78" s="82"/>
+      <c r="C78" s="82"/>
+      <c r="D78" s="83"/>
+      <c r="E78" s="84"/>
     </row>
     <row r="79" spans="1:6" ht="18" customHeight="1">
-      <c r="E79" s="25"/>
+      <c r="A79" s="85"/>
+      <c r="B79" s="86" t="s">
+        <v>4</v>
+      </c>
+      <c r="C79" s="86" t="s">
+        <v>5</v>
+      </c>
+      <c r="D79" s="86" t="s">
+        <v>6</v>
+      </c>
+      <c r="E79" s="86" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="80" spans="1:6" ht="18" customHeight="1">
       <c r="C80" s="25"/>
@@ -2801,28 +2751,9 @@
       <c r="D269" s="25"/>
       <c r="E269" s="25"/>
     </row>
-    <row r="270" spans="3:5" ht="18" customHeight="1">
-      <c r="C270" s="25"/>
-      <c r="D270" s="25"/>
-      <c r="E270" s="25"/>
-    </row>
-    <row r="271" spans="3:5" ht="18" customHeight="1">
-      <c r="C271" s="25"/>
-      <c r="D271" s="25"/>
-      <c r="E271" s="25"/>
-    </row>
-    <row r="272" spans="3:5" ht="18" customHeight="1">
-      <c r="C272" s="25"/>
-      <c r="D272" s="25"/>
-      <c r="E272" s="25"/>
-    </row>
-    <row r="273" spans="3:5" ht="18" customHeight="1">
-      <c r="C273" s="25"/>
-      <c r="D273" s="25"/>
-      <c r="E273" s="25"/>
-    </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="17">
+    <mergeCell ref="A78:D78"/>
     <mergeCell ref="A76:B76"/>
     <mergeCell ref="A63:D63"/>
     <mergeCell ref="A72:D72"/>

</xml_diff>